<commit_message>
pushing latest to github
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Key</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t>https://acme-test.uipath.com/work-items/update/</t>
+  </si>
+  <si>
+    <t>sha_url</t>
+  </si>
+  <si>
+    <t>http://www.sha1-online.com/</t>
   </si>
 </sst>
 </file>
@@ -45,7 +51,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,6 +64,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -88,12 +101,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -401,14 +417,14 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="18.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="73.14785714285713" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="19.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="73.14785714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -443,6 +459,14 @@
         <v>7</v>
       </c>
     </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>